<commit_message>
update angular newest version
Minor doc changes
</commit_message>
<xml_diff>
--- a/src/assets/upload_examples/accessions.xlsx
+++ b/src/assets/upload_examples/accessions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="73">
   <si>
     <t xml:space="preserve">INSTCODE</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">CONSTATUS</t>
   </si>
   <si>
+    <t xml:space="preserve">IN_NUCLEAR_COLLECTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">IS_AVAILABLE</t>
   </si>
   <si>
@@ -136,6 +139,9 @@
     <t xml:space="preserve">is_active</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
     <t xml:space="preserve">False</t>
   </si>
   <si>
@@ -185,9 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">CIAM81001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">ESP026</t>
@@ -242,14 +245,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -309,8 +314,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,51 +344,49 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="62.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="25.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="62.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="25.74"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -388,7 +399,7 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -480,355 +491,370 @@
       </c>
       <c r="AI1" s="0" t="s">
         <v>34</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>81001</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="L2" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="N2" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="O2" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="Q2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="0" t="n">
         <v>1840</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="X2" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="Y2" s="0" t="n">
         <v>19811031</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="AA2" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="AA2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB2" s="0" t="n">
+      <c r="AB2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="AE2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>52</v>
+      <c r="AF2" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="F3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>81001</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>1840</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>19811031</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI3" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>81001</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>1840</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>101</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>19811031</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z3" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="AA3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="AE3" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH3" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>81002</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="H4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="L4" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="N4" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="O4" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="Q4" s="0" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="W4" s="0" t="n">
+      <c r="X4" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="Y4" s="0" t="n">
         <v>19811031</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="AA4" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="AA4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB4" s="0" t="n">
+      <c r="AB4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="AE4" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH4" s="0" t="s">
-        <v>52</v>
+      <c r="AF4" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="AI4" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="AJ4" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>81002</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="H5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="L5" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="N5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="O5" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="Q5" s="0" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="W5" s="0" t="n">
+      <c r="X5" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="X5" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z5" s="0" t="n">
+      <c r="Y5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA5" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="AA5" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB5" s="0" t="n">
+      <c r="AB5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="AE5" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH5" s="0" t="s">
+      <c r="AF5" s="0" t="s">
         <v>64</v>
+      </c>
+      <c r="AI5" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>81003</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="L6" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="N6" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="O6" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="Q6" s="0" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="R6" s="0" t="s">
         <v>67</v>
@@ -836,73 +862,76 @@
       <c r="S6" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="T6" s="0" t="n">
+      <c r="T6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="U6" s="0" t="n">
         <v>1840</v>
       </c>
-      <c r="W6" s="0" t="n">
+      <c r="X6" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="X6" s="0" t="n">
+      <c r="Y6" s="0" t="n">
         <v>19811031</v>
       </c>
-      <c r="Z6" s="0" t="n">
+      <c r="AA6" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="AA6" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB6" s="0" t="n">
+      <c r="AB6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC6" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="AE6" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH6" s="0" t="s">
-        <v>64</v>
+      <c r="AF6" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>81003</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="H7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="N7" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="P7" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="O7" s="0" t="s">
+        <v>47</v>
+      </c>
       <c r="Q7" s="0" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="R7" s="0" t="s">
         <v>67</v>
@@ -910,26 +939,29 @@
       <c r="S7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="T7" s="0" t="n">
+      <c r="T7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="U7" s="0" t="n">
         <v>1840</v>
       </c>
-      <c r="W7" s="0" t="n">
+      <c r="X7" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="X7" s="0" t="n">
+      <c r="Y7" s="0" t="n">
         <v>19811031</v>
       </c>
-      <c r="Z7" s="0" t="n">
+      <c r="AA7" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="AA7" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB7" s="0" t="n">
+      <c r="AB7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC7" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="AE7" s="0" t="s">
-        <v>71</v>
+      <c r="AF7" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>